<commit_message>
modify UF_HWQUPC for assignment 3
</commit_message>
<xml_diff>
--- a/report/assign2/YueFang_AssignmentNo2.xlsx
+++ b/report/assign2/YueFang_AssignmentNo2.xlsx
@@ -5,21 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolWorks\NEU\INFO 6205\assign2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolWorks\NEU\INFO 6205\assign2\INFO6205\report\assign2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA4323A-5928-4991-95E9-9606317AA1F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BF30E1-6658-4A85-BB66-CCEBBC12403B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$21</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -244,7 +239,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$24</c:f>
+              <c:f>Sheet1!$G$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -267,7 +262,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$24:$M$24</c:f>
+              <c:f>Sheet1!$H$26:$M$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -304,7 +299,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$25</c:f>
+              <c:f>Sheet1!$G$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -327,7 +322,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$25:$M$25</c:f>
+              <c:f>Sheet1!$H$29:$M$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -364,7 +359,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$26</c:f>
+              <c:f>Sheet1!$G$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -387,7 +382,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$26:$M$26</c:f>
+              <c:f>Sheet1!$H$32:$M$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3418,16 +3413,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3454,16 +3449,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>652462</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>100012</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3792,8 +3787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4316,27 +4311,6 @@
       <c r="D24">
         <v>5000</v>
       </c>
-      <c r="G24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24">
-        <v>53.9</v>
-      </c>
-      <c r="I24">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="J24">
-        <v>43.174999999999997</v>
-      </c>
-      <c r="K24">
-        <v>51.862499999999997</v>
-      </c>
-      <c r="L24">
-        <v>42.143749999999997</v>
-      </c>
-      <c r="M24">
-        <v>42.556249999999999</v>
-      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -4351,27 +4325,6 @@
       <c r="D25">
         <v>5000</v>
       </c>
-      <c r="G25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25">
-        <v>116.2</v>
-      </c>
-      <c r="I25">
-        <v>112.65</v>
-      </c>
-      <c r="J25">
-        <v>109.5</v>
-      </c>
-      <c r="K25">
-        <v>117.425</v>
-      </c>
-      <c r="L25">
-        <v>109.66875</v>
-      </c>
-      <c r="M25">
-        <v>110.06874999999999</v>
-      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -4387,25 +4340,25 @@
         <v>5000</v>
       </c>
       <c r="G26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H26">
-        <v>40.4</v>
+        <v>53.9</v>
       </c>
       <c r="I26">
-        <v>43.75</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="J26">
-        <v>61.524999999999999</v>
+        <v>43.174999999999997</v>
       </c>
       <c r="K26">
-        <v>44.075000000000003</v>
+        <v>51.862499999999997</v>
       </c>
       <c r="L26">
-        <v>42.018749999999997</v>
+        <v>42.143749999999997</v>
       </c>
       <c r="M26">
-        <v>41.556249999999999</v>
+        <v>42.556249999999999</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -4449,6 +4402,27 @@
       <c r="D29">
         <v>5000</v>
       </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>116.2</v>
+      </c>
+      <c r="I29">
+        <v>112.65</v>
+      </c>
+      <c r="J29">
+        <v>109.5</v>
+      </c>
+      <c r="K29">
+        <v>117.425</v>
+      </c>
+      <c r="L29">
+        <v>109.66875</v>
+      </c>
+      <c r="M29">
+        <v>110.06874999999999</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -4490,6 +4464,27 @@
       </c>
       <c r="D32">
         <v>5000</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>40.4</v>
+      </c>
+      <c r="I32">
+        <v>43.75</v>
+      </c>
+      <c r="J32">
+        <v>61.524999999999999</v>
+      </c>
+      <c r="K32">
+        <v>44.075000000000003</v>
+      </c>
+      <c r="L32">
+        <v>42.018749999999997</v>
+      </c>
+      <c r="M32">
+        <v>41.556249999999999</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -5082,13 +5077,13 @@
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21 A23:A46 G23:G26 G15:G18 A48:A67 G49:G52" xr:uid="{D9B3F136-FE9D-4D82-801B-A3E3B340F77D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21 A23:A46 G15:G18 A48:A67 G49:G52 G23 G26 G32 G29" xr:uid="{D9B3F136-FE9D-4D82-801B-A3E3B340F77D}">
       <formula1>$G$2:$G$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B21 B24:B38 I22:K22 J14:L14 B53:B67 J48:L48" xr:uid="{245F4A41-3C55-47B8-AEA8-515F27FE6A90}">
       <formula1>$H$2:$H$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B23 B39:B46 G27:G28 H22 L22:M22 I14 M14 B48:B52 I48" xr:uid="{CEC7FF07-4455-440A-BC1F-641176AF4DE6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B23 B39:B46 H22 L22:M22 I14 M14 B48:B52 I48" xr:uid="{CEC7FF07-4455-440A-BC1F-641176AF4DE6}">
       <formula1>$H$2:$H$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>